<commit_message>
created updatePrices xls to json utils & index
</commit_message>
<xml_diff>
--- a/costofinal.xlsx
+++ b/costofinal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PAGINA DE INICIO" sheetId="1" state="visible" r:id="rId2"/>
@@ -1380,7 +1380,7 @@
     <t xml:space="preserve">TEURO30</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro  30 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 30 cm</t>
   </si>
   <si>
     <t xml:space="preserve">Termocuplas solas</t>
@@ -1389,31 +1389,31 @@
     <t xml:space="preserve">TEURO50</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro 50 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 50 cm</t>
   </si>
   <si>
     <t xml:space="preserve">TEURO60</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro 60 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 60 cm</t>
   </si>
   <si>
     <t xml:space="preserve">TEURO70</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro 70 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 70 cm</t>
   </si>
   <si>
     <t xml:space="preserve">TEURO80</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro 80 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 80 cm</t>
   </si>
   <si>
     <t xml:space="preserve">TEURO90</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas   Euro 90 cm</t>
+    <t xml:space="preserve">Termocuplas Euro 90 cm</t>
   </si>
   <si>
     <t xml:space="preserve">TSM820</t>
@@ -1437,7 +1437,7 @@
     <t xml:space="preserve">TSOU40</t>
   </si>
   <si>
-    <t xml:space="preserve">Termocuplas  simil Soporte Orbis Universal</t>
+    <t xml:space="preserve">Termocuplas simil Soporte Orbis Universal</t>
   </si>
   <si>
     <t xml:space="preserve">TSEGUER100</t>
@@ -3578,8 +3578,8 @@
   </sheetPr>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3727,7 +3727,6 @@
       <c r="G5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="0"/>
       <c r="I5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3750,7 +3749,6 @@
       <c r="G6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="0"/>
       <c r="I6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3784,7 +3782,6 @@
       <c r="C8" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="0"/>
       <c r="E8" s="15"/>
       <c r="F8" s="9" t="s">
         <v>46</v>
@@ -3805,7 +3802,6 @@
       <c r="C9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="0"/>
       <c r="E9" s="11"/>
       <c r="F9" s="9" t="s">
         <v>47</v>
@@ -3826,7 +3822,6 @@
       <c r="C10" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="0"/>
       <c r="E10" s="11"/>
       <c r="F10" s="9" t="s">
         <v>37</v>
@@ -3847,8 +3842,6 @@
       <c r="C11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
       <c r="F11" s="9" t="s">
         <v>56</v>
       </c>
@@ -3868,8 +3861,6 @@
       <c r="C12" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="0"/>
-      <c r="E12" s="0"/>
       <c r="F12" s="9" t="s">
         <v>61</v>
       </c>
@@ -3885,7 +3876,6 @@
         <v>63</v>
       </c>
       <c r="D13" s="17"/>
-      <c r="E13" s="0"/>
       <c r="F13" s="16" t="s">
         <v>64</v>
       </c>
@@ -3917,7 +3907,6 @@
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="0"/>
       <c r="G15" s="17"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -3929,7 +3918,6 @@
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="0"/>
       <c r="G16" s="17"/>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
@@ -3985,7 +3973,6 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17"/>
-      <c r="B21" s="0"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -3996,7 +3983,6 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="17"/>
-      <c r="B22" s="0"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -6265,7 +6251,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6298,7 +6284,7 @@
       <c r="C2" s="49" t="n">
         <v>259.813125</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6312,7 +6298,7 @@
       <c r="C3" s="49" t="n">
         <v>198.12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6326,7 +6312,7 @@
       <c r="C4" s="49" t="n">
         <v>263.68875</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6340,7 +6326,7 @@
       <c r="C5" s="49" t="n">
         <v>215.466875</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6354,7 +6340,7 @@
       <c r="C6" s="49" t="n">
         <v>223.738125</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6368,7 +6354,7 @@
       <c r="C7" s="49" t="n">
         <v>267.5725</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6382,7 +6368,7 @@
       <c r="C8" s="49" t="n">
         <v>195.495625</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6396,7 +6382,7 @@
       <c r="C9" s="49" t="n">
         <v>242.4825</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6410,7 +6396,7 @@
       <c r="C10" s="49" t="n">
         <v>294.636875</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6424,7 +6410,7 @@
       <c r="C11" s="49" t="n">
         <v>314.68125</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6438,7 +6424,7 @@
       <c r="C12" s="49" t="n">
         <v>333.43375</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6452,7 +6438,7 @@
       <c r="C13" s="49" t="n">
         <v>378.763125</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6466,7 +6452,7 @@
       <c r="C14" s="49" t="n">
         <v>290.82625</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6480,7 +6466,7 @@
       <c r="C15" s="49" t="n">
         <v>322.326875</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6494,7 +6480,7 @@
       <c r="C16" s="49" t="n">
         <v>287.67375</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6508,7 +6494,7 @@
       <c r="C17" s="49" t="n">
         <v>307.100625</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6522,7 +6508,7 @@
       <c r="C18" s="49" t="n">
         <v>284.350625</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6536,7 +6522,7 @@
       <c r="C19" s="49" t="n">
         <v>311.211875</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6550,7 +6536,7 @@
       <c r="C20" s="49" t="n">
         <v>289.49375</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6564,7 +6550,7 @@
       <c r="C21" s="49" t="n">
         <v>289.49375</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6578,7 +6564,7 @@
       <c r="C22" s="49" t="n">
         <v>294.051875</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6592,7 +6578,7 @@
       <c r="C23" s="49" t="n">
         <v>294.051875</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6606,7 +6592,7 @@
       <c r="C24" s="49" t="n">
         <v>287.67375</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6620,7 +6606,7 @@
       <c r="C25" s="49" t="n">
         <v>280.450625</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6634,7 +6620,7 @@
       <c r="C26" s="49" t="n">
         <v>244.35125</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6648,7 +6634,7 @@
       <c r="C27" s="49" t="n">
         <v>300.941875</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6662,7 +6648,7 @@
       <c r="C28" s="49" t="n">
         <v>311.211875</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6676,7 +6662,7 @@
       <c r="C29" s="49" t="n">
         <v>311.211875</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6690,7 +6676,7 @@
       <c r="C30" s="49" t="n">
         <v>215.466875</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>389</v>
       </c>
     </row>
@@ -6704,7 +6690,7 @@
       <c r="C31" s="49" t="n">
         <v>352.86875</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6718,7 +6704,7 @@
       <c r="C32" s="49" t="n">
         <v>250.680625</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6732,7 +6718,7 @@
       <c r="C33" s="49" t="n">
         <v>341.10375</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6746,7 +6732,7 @@
       <c r="C34" s="49" t="n">
         <v>283.765625</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6760,7 +6746,7 @@
       <c r="C35" s="49" t="n">
         <v>317.785</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6774,7 +6760,7 @@
       <c r="C36" s="49" t="n">
         <v>414.06625</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6788,7 +6774,7 @@
       <c r="C37" s="49" t="n">
         <v>267.085</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6802,7 +6788,7 @@
       <c r="C38" s="49" t="n">
         <v>235.7875</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>444</v>
       </c>
     </row>
@@ -6816,7 +6802,7 @@
       <c r="C39" s="49" t="n">
         <v>91.2060826060606</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>447</v>
       </c>
     </row>
@@ -6838,8 +6824,8 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6872,7 +6858,7 @@
       <c r="C2" s="49" t="n">
         <v>424.56</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6886,7 +6872,7 @@
       <c r="C3" s="49" t="n">
         <v>526.82</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6900,7 +6886,7 @@
       <c r="C4" s="49" t="n">
         <v>564</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6914,7 +6900,7 @@
       <c r="C5" s="49" t="n">
         <v>594.86</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6928,7 +6914,7 @@
       <c r="C6" s="49" t="n">
         <v>635.3</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6942,7 +6928,7 @@
       <c r="C7" s="49" t="n">
         <v>678.84</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6956,7 +6942,7 @@
       <c r="C8" s="49" t="n">
         <v>469.63</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6970,7 +6956,7 @@
       <c r="C9" s="49" t="n">
         <v>692.74</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6981,7 +6967,7 @@
       <c r="C10" s="49" t="n">
         <v>424.56</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6992,7 +6978,7 @@
       <c r="C11" s="49" t="n">
         <v>564</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7006,7 +6992,7 @@
       <c r="C12" s="49" t="n">
         <v>486.5</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7020,7 +7006,7 @@
       <c r="C13" s="49" t="n">
         <v>712.77</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7034,7 +7020,7 @@
       <c r="C14" s="49" t="n">
         <v>578.142208</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7048,7 +7034,7 @@
       <c r="C15" s="49" t="n">
         <v>608.147456</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7062,7 +7048,7 @@
       <c r="C16" s="49" t="n">
         <v>691.862528</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7076,7 +7062,7 @@
       <c r="C17" s="49" t="n">
         <v>785.6128</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7090,7 +7076,7 @@
       <c r="C18" s="49" t="n">
         <v>879.37024</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7104,7 +7090,7 @@
       <c r="C19" s="49" t="n">
         <v>973.12768</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7118,7 +7104,7 @@
       <c r="C20" s="49" t="n">
         <v>1066.906624</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7132,7 +7118,7 @@
       <c r="C21" s="49" t="n">
         <v>1255.86944</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7146,7 +7132,7 @@
       <c r="C22" s="49" t="n">
         <v>1336.86784</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7160,7 +7146,7 @@
       <c r="C23" s="49" t="n">
         <v>1446.695936</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7174,7 +7160,7 @@
       <c r="C24" s="49" t="n">
         <v>1542.367232</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7188,7 +7174,7 @@
       <c r="C25" s="49" t="n">
         <v>1734.290432</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>473</v>
       </c>
     </row>
@@ -7202,7 +7188,7 @@
       <c r="C26" s="49" t="n">
         <v>834.885632</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7216,7 +7202,7 @@
       <c r="C27" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7230,7 +7216,7 @@
       <c r="C28" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7244,7 +7230,7 @@
       <c r="C29" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7258,7 +7244,7 @@
       <c r="C30" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7272,7 +7258,7 @@
       <c r="C31" s="49" t="n">
         <v>173.917184</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7286,7 +7272,7 @@
       <c r="C32" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7300,7 +7286,7 @@
       <c r="C33" s="49" t="n">
         <v>124.450816</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7314,7 +7300,7 @@
       <c r="C34" s="49" t="n">
         <v>145.316864</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>501</v>
       </c>
     </row>
@@ -7328,7 +7314,7 @@
       <c r="C35" s="49" t="n">
         <v>53.279744</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7342,7 +7328,7 @@
       <c r="C36" s="49" t="n">
         <v>53.279744</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7356,7 +7342,7 @@
       <c r="C37" s="49" t="n">
         <v>53.279744</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7370,7 +7356,7 @@
       <c r="C38" s="49" t="n">
         <v>53.279744</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7384,7 +7370,7 @@
       <c r="C39" s="49" t="n">
         <v>70.884352</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7398,7 +7384,7 @@
       <c r="C40" s="49" t="n">
         <v>34.671616</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7412,7 +7398,7 @@
       <c r="C41" s="49" t="n">
         <v>63.18</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>321</v>
       </c>
     </row>
@@ -7426,7 +7412,7 @@
       <c r="C42" s="49" t="n">
         <v>489.276928</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7440,7 +7426,7 @@
       <c r="C43" s="49" t="n">
         <v>519.282176</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7454,7 +7440,7 @@
       <c r="C44" s="49" t="n">
         <v>602.997248</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7468,7 +7454,7 @@
       <c r="C45" s="49" t="n">
         <v>696.74752</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7482,7 +7468,7 @@
       <c r="C46" s="49" t="n">
         <v>790.50496</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7496,7 +7482,7 @@
       <c r="C47" s="49" t="n">
         <v>884.2624</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7510,7 +7496,7 @@
       <c r="C48" s="49" t="n">
         <v>978.041344</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7524,7 +7510,7 @@
       <c r="C49" s="49" t="n">
         <v>1167.00416</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7538,7 +7524,7 @@
       <c r="C50" s="49" t="n">
         <v>1357.830656</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7552,7 +7538,7 @@
       <c r="C51" s="49" t="n">
         <v>1645.425152</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>498</v>
       </c>
     </row>
@@ -7608,7 +7594,7 @@
       <c r="C2" s="49" t="n">
         <v>11.37162</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>551</v>
       </c>
     </row>
@@ -7622,7 +7608,7 @@
       <c r="C3" s="49" t="n">
         <v>16.62128</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>551</v>
       </c>
     </row>
@@ -7636,7 +7622,7 @@
       <c r="C4" s="49" t="n">
         <v>23.16353</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>551</v>
       </c>
     </row>
@@ -7650,7 +7636,7 @@
       <c r="C5" s="49" t="n">
         <v>11.38748</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7664,7 +7650,7 @@
       <c r="C6" s="49" t="n">
         <v>17.96145</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7678,7 +7664,7 @@
       <c r="C7" s="49" t="n">
         <v>25.16189</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7692,7 +7678,7 @@
       <c r="C8" s="49" t="n">
         <v>23.34592</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7706,7 +7692,7 @@
       <c r="C9" s="49" t="n">
         <v>32.90157</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7720,7 +7706,7 @@
       <c r="C10" s="49" t="n">
         <v>41.7118</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7734,7 +7720,7 @@
       <c r="C11" s="49" t="n">
         <v>22.81461</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7748,7 +7734,7 @@
       <c r="C12" s="49" t="n">
         <v>30.26088</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7762,7 +7748,7 @@
       <c r="C13" s="49" t="n">
         <v>45.1217</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7776,7 +7762,7 @@
       <c r="C14" s="49" t="n">
         <v>35.93876</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7790,7 +7776,7 @@
       <c r="C15" s="49" t="n">
         <v>56.92154</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7804,7 +7790,7 @@
       <c r="C16" s="49" t="n">
         <v>74.39133</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7818,7 +7804,7 @@
       <c r="C17" s="49" t="n">
         <v>26.89856</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7832,7 +7818,7 @@
       <c r="C18" s="49" t="n">
         <v>39.14248</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7846,7 +7832,7 @@
       <c r="C19" s="49" t="n">
         <v>74.51821</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7860,7 +7846,7 @@
       <c r="C20" s="49" t="n">
         <v>28.18322</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7874,7 +7860,7 @@
       <c r="C21" s="49" t="n">
         <v>20.37217</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7888,7 +7874,7 @@
       <c r="C22" s="49" t="n">
         <v>21.38721</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7902,7 +7888,7 @@
       <c r="C23" s="49" t="n">
         <v>28.61144</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7916,7 +7902,7 @@
       <c r="C24" s="49" t="n">
         <v>28.61144</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7930,7 +7916,7 @@
       <c r="C25" s="49" t="n">
         <v>35.81981</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7944,7 +7930,7 @@
       <c r="C26" s="49" t="n">
         <v>41.17256</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7958,7 +7944,7 @@
       <c r="C27" s="49" t="n">
         <v>41.17256</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7972,7 +7958,7 @@
       <c r="C28" s="49" t="n">
         <v>41.17256</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -7986,7 +7972,7 @@
       <c r="C29" s="49" t="n">
         <v>41.17256</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -8000,7 +7986,7 @@
       <c r="C30" s="49" t="n">
         <v>41.17256</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>558</v>
       </c>
     </row>
@@ -8014,7 +8000,7 @@
       <c r="C31" s="49" t="n">
         <v>19.34127</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>611</v>
       </c>
     </row>
@@ -8028,7 +8014,7 @@
       <c r="C32" s="49" t="n">
         <v>25.62183</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>611</v>
       </c>
     </row>
@@ -8042,7 +8028,7 @@
       <c r="C33" s="49" t="n">
         <v>25.62183</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>611</v>
       </c>
     </row>
@@ -8056,7 +8042,7 @@
       <c r="C34" s="49" t="n">
         <v>33.02845</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8070,7 +8056,7 @@
       <c r="C35" s="49" t="n">
         <v>42.59996</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8084,7 +8070,7 @@
       <c r="C36" s="49" t="n">
         <v>71.04487</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8098,7 +8084,7 @@
       <c r="C37" s="49" t="n">
         <v>59.80806</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8112,7 +8098,7 @@
       <c r="C38" s="49" t="n">
         <v>69.4668</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8126,7 +8112,7 @@
       <c r="C39" s="49" t="n">
         <v>91.96421</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8140,7 +8126,7 @@
       <c r="C40" s="49" t="n">
         <v>55.51793</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8154,7 +8140,7 @@
       <c r="C41" s="49" t="n">
         <v>65.71591</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8168,7 +8154,7 @@
       <c r="C42" s="49" t="n">
         <v>93.70088</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>618</v>
       </c>
     </row>
@@ -8224,7 +8210,7 @@
       <c r="C2" s="49" t="n">
         <v>20.55375</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>637</v>
       </c>
     </row>
@@ -8238,7 +8224,7 @@
       <c r="C3" s="49" t="n">
         <v>21.853125</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8252,7 +8238,7 @@
       <c r="C4" s="49" t="n">
         <v>30.79125</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8266,7 +8252,7 @@
       <c r="C5" s="49" t="n">
         <v>54.0225</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8280,7 +8266,7 @@
       <c r="C6" s="49" t="n">
         <v>35.316</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8294,7 +8280,7 @@
       <c r="C7" s="49" t="n">
         <v>55.902</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8308,7 +8294,7 @@
       <c r="C8" s="49" t="n">
         <v>38.1375</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8322,7 +8308,7 @@
       <c r="C9" s="49" t="n">
         <v>84.72</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8336,7 +8322,7 @@
       <c r="C10" s="49" t="n">
         <v>66.725</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -8350,7 +8336,7 @@
       <c r="C11" s="49" t="n">
         <v>19.13625</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8364,7 +8350,7 @@
       <c r="C12" s="49" t="n">
         <v>24.215625</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8378,7 +8364,7 @@
       <c r="C13" s="49" t="n">
         <v>31.303125</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8392,7 +8378,7 @@
       <c r="C14" s="49" t="n">
         <v>23.270625</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8406,7 +8392,7 @@
       <c r="C15" s="49" t="n">
         <v>34.825</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8420,7 +8406,7 @@
       <c r="C16" s="49" t="n">
         <v>29.570625</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8434,7 +8420,7 @@
       <c r="C17" s="49" t="n">
         <v>95.1</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>668</v>
       </c>
     </row>
@@ -8448,7 +8434,7 @@
       <c r="C18" s="49" t="n">
         <v>123.625</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>668</v>
       </c>
     </row>
@@ -8462,7 +8448,7 @@
       <c r="C19" s="49" t="n">
         <v>27.64125</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8476,7 +8462,7 @@
       <c r="C20" s="49" t="n">
         <v>35.91</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8490,7 +8476,7 @@
       <c r="C21" s="49" t="n">
         <v>63.590625</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8504,7 +8490,7 @@
       <c r="C22" s="49" t="n">
         <v>49.8875</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8518,7 +8504,7 @@
       <c r="C23" s="49" t="n">
         <v>107.652</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8532,7 +8518,7 @@
       <c r="C24" s="49" t="n">
         <v>81.125</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -8546,7 +8532,7 @@
       <c r="C25" s="49" t="n">
         <v>17.994375</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -8560,7 +8546,7 @@
       <c r="C26" s="49" t="n">
         <v>21.49875</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -8574,7 +8560,7 @@
       <c r="C27" s="49" t="n">
         <v>29.295</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -8588,7 +8574,7 @@
       <c r="C28" s="49" t="n">
         <v>122.5875</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>691</v>
       </c>
     </row>
@@ -8602,7 +8588,7 @@
       <c r="C29" s="49" t="n">
         <v>131.9375</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>691</v>
       </c>
     </row>
@@ -8616,7 +8602,7 @@
       <c r="C30" s="49" t="n">
         <v>188.55</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>691</v>
       </c>
     </row>
@@ -8630,7 +8616,7 @@
       <c r="C31" s="49" t="n">
         <v>180.975</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>698</v>
       </c>
     </row>
@@ -8644,7 +8630,7 @@
       <c r="C32" s="49" t="n">
         <v>247.536</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>698</v>
       </c>
     </row>
@@ -8658,7 +8644,7 @@
       <c r="C33" s="49" t="n">
         <v>396.234</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>698</v>
       </c>
     </row>
@@ -8670,7 +8656,7 @@
         <v>704</v>
       </c>
       <c r="C34" s="49"/>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8684,7 +8670,7 @@
       <c r="C35" s="49" t="n">
         <v>244.9125</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8698,7 +8684,7 @@
       <c r="C36" s="49" t="n">
         <v>343.58625</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8712,7 +8698,7 @@
       <c r="C37" s="49" t="n">
         <v>257.67</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8726,7 +8712,7 @@
       <c r="C38" s="49" t="n">
         <v>344.1375</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8740,7 +8726,7 @@
       <c r="C39" s="49" t="n">
         <v>679.8</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8754,7 +8740,7 @@
       <c r="C40" s="49" t="n">
         <v>336.105</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8768,7 +8754,7 @@
       <c r="C41" s="49" t="n">
         <v>455.450625</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8782,7 +8768,7 @@
       <c r="C42" s="49" t="n">
         <v>343.5075</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8796,7 +8782,7 @@
       <c r="C43" s="49" t="n">
         <v>456.12</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8810,7 +8796,7 @@
       <c r="C44" s="49" t="n">
         <v>776.916</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8824,7 +8810,7 @@
       <c r="C45" s="49" t="n">
         <v>874.032</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>705</v>
       </c>
     </row>
@@ -8838,7 +8824,7 @@
       <c r="C46" s="49" t="n">
         <v>251.37</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8852,7 +8838,7 @@
       <c r="C47" s="49" t="n">
         <v>412.734</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8866,7 +8852,7 @@
       <c r="C48" s="49" t="n">
         <v>278.22375</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8880,7 +8866,7 @@
       <c r="C49" s="49" t="n">
         <v>410.59998</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8894,7 +8880,7 @@
       <c r="C50" s="49" t="n">
         <v>576.7875</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8908,7 +8894,7 @@
       <c r="C51" s="49" t="n">
         <v>812.214</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8922,7 +8908,7 @@
       <c r="C52" s="49" t="n">
         <v>343.8225</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8936,7 +8922,7 @@
       <c r="C53" s="49" t="n">
         <v>534.126</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8950,7 +8936,7 @@
       <c r="C54" s="49" t="n">
         <v>363.6675</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8964,7 +8950,7 @@
       <c r="C55" s="49" t="n">
         <v>527.009112</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8978,7 +8964,7 @@
       <c r="C56" s="49" t="n">
         <v>874.032</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>730</v>
       </c>
     </row>
@@ -8992,7 +8978,7 @@
       <c r="C57" s="49" t="n">
         <v>285.46875</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9006,7 +8992,7 @@
       <c r="C58" s="49" t="n">
         <v>427.308</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9020,7 +9006,7 @@
       <c r="C59" s="49" t="n">
         <v>558.402</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9034,7 +9020,7 @@
       <c r="C60" s="49" t="n">
         <v>236.51352</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9048,7 +9034,7 @@
       <c r="C61" s="49" t="n">
         <v>376.11</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9062,7 +9048,7 @@
       <c r="C62" s="49" t="n">
         <v>534.018</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9076,7 +9062,7 @@
       <c r="C63" s="49" t="n">
         <v>631.248</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="1" t="s">
         <v>753</v>
       </c>
     </row>
@@ -9090,7 +9076,7 @@
       <c r="C64" s="49" t="n">
         <v>1866.6</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9104,7 +9090,7 @@
       <c r="C65" s="49" t="n">
         <v>2049.6</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9118,7 +9104,7 @@
       <c r="C66" s="49" t="n">
         <v>2232.6</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9132,7 +9118,7 @@
       <c r="C67" s="49" t="n">
         <v>414.8</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9146,7 +9132,7 @@
       <c r="C68" s="49" t="n">
         <v>646.6</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9160,7 +9146,7 @@
       <c r="C69" s="49" t="n">
         <v>976</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="1" t="s">
         <v>767</v>
       </c>
     </row>
@@ -9174,7 +9160,7 @@
       <c r="C70" s="49" t="n">
         <v>1476.2</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="1" t="s">
         <v>780</v>
       </c>
     </row>
@@ -9230,7 +9216,7 @@
       <c r="C2" s="49" t="n">
         <v>27.08355</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9244,7 +9230,7 @@
       <c r="C3" s="49" t="n">
         <v>44.4106</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9258,7 +9244,7 @@
       <c r="C4" s="49" t="n">
         <v>72.43275</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9272,7 +9258,7 @@
       <c r="C5" s="49" t="n">
         <v>28.9731</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9286,7 +9272,7 @@
       <c r="C6" s="49" t="n">
         <v>44.0895</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9300,7 +9286,7 @@
       <c r="C7" s="49" t="n">
         <v>27.7134</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -9314,7 +9300,7 @@
       <c r="C8" s="49" t="n">
         <v>40.3104</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -9328,7 +9314,7 @@
       <c r="C9" s="49" t="n">
         <v>62.985</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -9342,7 +9328,7 @@
       <c r="C10" s="49" t="n">
         <v>37.791</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>83</v>
       </c>
     </row>
@@ -9356,7 +9342,7 @@
       <c r="C11" s="49" t="n">
         <v>62.985</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>668</v>
       </c>
     </row>
@@ -9370,7 +9356,7 @@
       <c r="C12" s="49" t="n">
         <v>88.179</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>668</v>
       </c>
     </row>
@@ -9384,7 +9370,7 @@
       <c r="C13" s="49" t="n">
         <v>119.6715</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>805</v>
       </c>
     </row>
@@ -9398,7 +9384,7 @@
       <c r="C14" s="49" t="n">
         <v>127.2297</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>805</v>
       </c>
     </row>
@@ -9412,7 +9398,7 @@
       <c r="C15" s="49" t="n">
         <v>178.24755</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>805</v>
       </c>
     </row>
@@ -9426,7 +9412,7 @@
       <c r="C16" s="49" t="n">
         <v>44.0895</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -9440,7 +9426,7 @@
       <c r="C17" s="49" t="n">
         <v>78.73125</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -9454,7 +9440,7 @@
       <c r="C18" s="49" t="n">
         <v>119.6715</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -9468,7 +9454,7 @@
       <c r="C19" s="49" t="n">
         <v>22.6746</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>815</v>
       </c>
     </row>
@@ -9482,7 +9468,7 @@
       <c r="C20" s="49" t="n">
         <v>27.7134</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>815</v>
       </c>
     </row>
@@ -9496,7 +9482,7 @@
       <c r="C21" s="49" t="n">
         <v>30.2328</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>815</v>
       </c>
     </row>
@@ -9510,7 +9496,7 @@
       <c r="C22" s="49" t="n">
         <v>20.78505</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9524,7 +9510,7 @@
       <c r="C23" s="49" t="n">
         <v>24.56415</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9538,7 +9524,7 @@
       <c r="C24" s="49" t="n">
         <v>31.4925</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9552,7 +9538,7 @@
       <c r="C25" s="49" t="n">
         <v>27.7134</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9566,7 +9552,7 @@
       <c r="C26" s="49" t="n">
         <v>32.7522</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9580,7 +9566,7 @@
       <c r="C27" s="49" t="n">
         <v>32.7522</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9594,7 +9580,7 @@
       <c r="C28" s="49" t="n">
         <v>20.1552</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -9608,7 +9594,7 @@
       <c r="C29" s="49" t="n">
         <v>20.1552</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -9622,7 +9608,7 @@
       <c r="C30" s="49" t="n">
         <v>25.194</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -9636,7 +9622,7 @@
       <c r="C31" s="49" t="n">
         <v>25.194</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -9650,7 +9636,7 @@
       <c r="C32" s="49" t="n">
         <v>28.34325</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -9664,7 +9650,7 @@
       <c r="C33" s="49" t="n">
         <v>37.791</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -9678,7 +9664,7 @@
       <c r="C34" s="49" t="n">
         <v>17.69</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9692,7 +9678,7 @@
       <c r="C35" s="49" t="n">
         <v>23.79</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9706,7 +9692,7 @@
       <c r="C36" s="49" t="n">
         <v>29.28</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9720,7 +9706,7 @@
       <c r="C37" s="49" t="n">
         <v>32.94</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9734,7 +9720,7 @@
       <c r="C38" s="49" t="n">
         <v>39.04</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9748,7 +9734,7 @@
       <c r="C39" s="49" t="n">
         <v>53.07</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9762,7 +9748,7 @@
       <c r="C40" s="49" t="n">
         <v>21.96</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9776,7 +9762,7 @@
       <c r="C41" s="49" t="n">
         <v>31.11</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9790,7 +9776,7 @@
       <c r="C42" s="49" t="n">
         <v>39.04</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9804,7 +9790,7 @@
       <c r="C43" s="49" t="n">
         <v>46.36</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9818,7 +9804,7 @@
       <c r="C44" s="49" t="n">
         <v>57.34</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9832,7 +9818,7 @@
       <c r="C45" s="49" t="n">
         <v>69.54</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9846,7 +9832,7 @@
       <c r="C46" s="49" t="n">
         <v>32.94</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9860,7 +9846,7 @@
       <c r="C47" s="49" t="n">
         <v>43.92</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9874,7 +9860,7 @@
       <c r="C48" s="49" t="n">
         <v>57.95</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9888,7 +9874,7 @@
       <c r="C49" s="49" t="n">
         <v>70.76</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9902,7 +9888,7 @@
       <c r="C50" s="49" t="n">
         <v>84.79</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9916,7 +9902,7 @@
       <c r="C51" s="49" t="n">
         <v>96.38</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9972,7 +9958,7 @@
       <c r="C2" s="49" t="n">
         <v>577.5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -9986,7 +9972,7 @@
       <c r="C3" s="49" t="n">
         <v>91.7125</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10000,7 +9986,7 @@
       <c r="C4" s="49" t="n">
         <v>91.7125</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10014,7 +10000,7 @@
       <c r="C5" s="49" t="n">
         <v>183.4375</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10028,7 +10014,7 @@
       <c r="C6" s="49" t="n">
         <v>183.4375</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10042,7 +10028,7 @@
       <c r="C7" s="49" t="n">
         <v>145.1</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10056,7 +10042,7 @@
       <c r="C8" s="49" t="n">
         <v>145.1</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10070,7 +10056,7 @@
       <c r="C9" s="49" t="n">
         <v>148.925</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>877</v>
       </c>
     </row>
@@ -10084,7 +10070,7 @@
       <c r="C10" s="49" t="n">
         <v>225</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10098,7 +10084,7 @@
       <c r="C11" s="49" t="n">
         <v>256.25</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10112,7 +10098,7 @@
       <c r="C12" s="49" t="n">
         <v>300</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10126,7 +10112,7 @@
       <c r="C13" s="49" t="n">
         <v>481.25</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10140,7 +10126,7 @@
       <c r="C14" s="49" t="n">
         <v>225</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -10154,7 +10140,7 @@
       <c r="C15" s="49" t="n">
         <v>256.25</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -10168,7 +10154,7 @@
       <c r="C16" s="49" t="n">
         <v>300</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -10182,7 +10168,7 @@
       <c r="C17" s="49" t="n">
         <v>481.25</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -10196,7 +10182,7 @@
       <c r="C18" s="49" t="n">
         <v>124.8</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10210,7 +10196,7 @@
       <c r="C19" s="49" t="n">
         <v>152.1</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>894</v>
       </c>
     </row>
@@ -10224,7 +10210,7 @@
       <c r="C20" s="49" t="n">
         <v>235.3</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>894</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change costofinal.xls adding KIT
</commit_message>
<xml_diff>
--- a/costofinal.xlsx
+++ b/costofinal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="PAGINA DE INICIO" sheetId="1" state="visible" r:id="rId2"/>
@@ -4038,7 +4038,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4312,7 +4312,7 @@
         <v>105</v>
       </c>
       <c r="E14" s="34" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F14" s="34"/>
     </row>
@@ -4331,7 +4331,7 @@
         <v>105</v>
       </c>
       <c r="E15" s="34" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F15" s="34"/>
     </row>
@@ -4737,7 +4737,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4754,7 +4754,7 @@
       <c r="D2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       <c r="D3" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4788,7 +4788,7 @@
       <c r="D4" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4805,7 +4805,7 @@
       <c r="D5" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       <c r="D6" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4839,7 +4839,7 @@
       <c r="D7" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4856,7 +4856,7 @@
       <c r="D8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4873,7 +4873,7 @@
       <c r="D9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4890,7 +4890,7 @@
       <c r="D10" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4907,7 +4907,7 @@
       <c r="D11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4924,7 +4924,7 @@
       <c r="D12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       <c r="D13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4958,7 +4958,7 @@
       <c r="D14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4975,7 +4975,7 @@
       <c r="D15" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -4992,7 +4992,7 @@
       <c r="D16" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5009,7 +5009,7 @@
       <c r="D17" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5026,7 +5026,7 @@
       <c r="D18" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5043,7 +5043,7 @@
       <c r="D19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5060,7 +5060,7 @@
       <c r="D20" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       <c r="D21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5094,7 +5094,7 @@
       <c r="D22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
       <c r="D23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5128,7 +5128,7 @@
       <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5145,7 +5145,7 @@
       <c r="D25" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
       <c r="D26" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5179,7 +5179,7 @@
       <c r="D27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5196,7 +5196,7 @@
       <c r="D28" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5213,7 +5213,7 @@
       <c r="D29" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5230,7 +5230,7 @@
       <c r="D30" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       <c r="D31" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
       <c r="D32" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5281,7 +5281,7 @@
       <c r="D33" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5298,7 +5298,7 @@
       <c r="D34" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5315,7 +5315,7 @@
       <c r="D35" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5332,7 +5332,7 @@
       <c r="D36" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       <c r="D37" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
       <c r="D38" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5383,7 +5383,7 @@
       <c r="D39" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5400,7 +5400,7 @@
       <c r="D40" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       <c r="D41" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5434,7 +5434,7 @@
       <c r="D42" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5451,7 +5451,7 @@
       <c r="D43" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5468,7 +5468,7 @@
       <c r="D44" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5485,7 +5485,7 @@
       <c r="D45" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5502,7 +5502,7 @@
       <c r="D46" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       <c r="D47" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5536,7 +5536,7 @@
       <c r="D48" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5553,7 +5553,7 @@
       <c r="D49" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5570,7 +5570,7 @@
       <c r="D50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       <c r="D51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5604,7 +5604,7 @@
       <c r="D52" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5621,7 +5621,7 @@
       <c r="D53" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5638,7 +5638,7 @@
       <c r="D54" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5655,7 +5655,7 @@
       <c r="D55" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5672,7 +5672,7 @@
       <c r="D56" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E56" s="0" t="n">
+      <c r="E56" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       <c r="D57" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5706,7 +5706,7 @@
       <c r="D58" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5723,7 +5723,7 @@
       <c r="D59" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5740,7 +5740,7 @@
       <c r="D60" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5757,7 +5757,7 @@
       <c r="D61" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5774,7 +5774,7 @@
       <c r="D62" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5791,7 +5791,7 @@
       <c r="D63" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5808,7 +5808,7 @@
       <c r="D64" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E64" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5825,7 +5825,7 @@
       <c r="D65" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E65" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5842,7 +5842,7 @@
       <c r="D66" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5859,7 +5859,7 @@
       <c r="D67" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       <c r="D68" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5893,7 +5893,7 @@
       <c r="D69" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5910,7 +5910,7 @@
       <c r="D70" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5927,7 +5927,7 @@
       <c r="D71" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E71" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5944,7 +5944,7 @@
       <c r="D72" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E72" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5961,7 +5961,7 @@
       <c r="D73" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E73" s="0" t="n">
+      <c r="E73" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5978,7 +5978,7 @@
       <c r="D74" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E74" s="0" t="n">
+      <c r="E74" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -5995,7 +5995,7 @@
       <c r="D75" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E75" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6012,7 +6012,7 @@
       <c r="D76" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="0" t="n">
+      <c r="E76" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6029,7 +6029,7 @@
       <c r="D77" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E77" s="0" t="n">
+      <c r="E77" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6046,7 +6046,7 @@
       <c r="D78" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E78" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6063,7 +6063,7 @@
       <c r="D79" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6080,7 +6080,7 @@
       <c r="D80" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E80" s="0" t="n">
+      <c r="E80" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6097,7 +6097,7 @@
       <c r="D81" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E81" s="0" t="n">
+      <c r="E81" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6114,7 +6114,7 @@
       <c r="D82" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E82" s="0" t="n">
+      <c r="E82" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       <c r="D83" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6148,7 +6148,7 @@
       <c r="D84" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E84" s="0" t="n">
+      <c r="E84" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6165,7 +6165,7 @@
       <c r="D85" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6182,7 +6182,7 @@
       <c r="D86" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E86" s="0" t="n">
+      <c r="E86" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6199,7 +6199,7 @@
       <c r="D87" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E87" s="0" t="n">
+      <c r="E87" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6216,7 +6216,7 @@
       <c r="D88" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E88" s="0" t="n">
+      <c r="E88" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6233,7 +6233,7 @@
       <c r="D89" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E89" s="0" t="n">
+      <c r="E89" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6250,7 +6250,7 @@
       <c r="D90" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E90" s="0" t="n">
+      <c r="E90" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6267,7 +6267,7 @@
       <c r="D91" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E91" s="0" t="n">
+      <c r="E91" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6284,7 +6284,7 @@
       <c r="D92" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E92" s="0" t="n">
+      <c r="E92" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6301,7 +6301,7 @@
       <c r="D93" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E93" s="0" t="n">
+      <c r="E93" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6318,7 +6318,7 @@
       <c r="D94" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E94" s="0" t="n">
+      <c r="E94" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6335,7 +6335,7 @@
       <c r="D95" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E95" s="0" t="n">
+      <c r="E95" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6352,7 +6352,7 @@
       <c r="D96" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E96" s="0" t="n">
+      <c r="E96" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6369,7 +6369,7 @@
       <c r="D97" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E97" s="0" t="n">
+      <c r="E97" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6386,7 +6386,7 @@
       <c r="D98" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E98" s="0" t="n">
+      <c r="E98" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6403,7 +6403,7 @@
       <c r="D99" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E99" s="0" t="n">
+      <c r="E99" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6420,7 +6420,7 @@
       <c r="D100" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E100" s="0" t="n">
+      <c r="E100" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6437,7 +6437,7 @@
       <c r="D101" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E101" s="0" t="n">
+      <c r="E101" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6454,7 +6454,7 @@
       <c r="D102" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E102" s="0" t="n">
+      <c r="E102" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6471,7 +6471,7 @@
       <c r="D103" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E103" s="0" t="n">
+      <c r="E103" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6488,7 +6488,7 @@
       <c r="D104" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E104" s="0" t="n">
+      <c r="E104" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6505,7 +6505,7 @@
       <c r="D105" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E105" s="0" t="n">
+      <c r="E105" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6522,7 +6522,7 @@
       <c r="D106" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E106" s="0" t="n">
+      <c r="E106" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6539,7 +6539,7 @@
       <c r="D107" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E107" s="0" t="n">
+      <c r="E107" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6556,7 +6556,7 @@
       <c r="D108" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E108" s="0" t="n">
+      <c r="E108" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6573,7 +6573,7 @@
       <c r="D109" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E109" s="0" t="n">
+      <c r="E109" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6590,7 +6590,7 @@
       <c r="D110" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E110" s="0" t="n">
+      <c r="E110" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6607,7 +6607,7 @@
       <c r="D111" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E111" s="0" t="n">
+      <c r="E111" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6624,7 +6624,7 @@
       <c r="D112" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E112" s="0" t="n">
+      <c r="E112" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6671,7 +6671,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -6688,7 +6688,7 @@
       <c r="D2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6705,7 +6705,7 @@
       <c r="D3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6722,7 +6722,7 @@
       <c r="D4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6739,7 +6739,7 @@
       <c r="D5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6756,7 +6756,7 @@
       <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6773,7 +6773,7 @@
       <c r="D7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6790,7 +6790,7 @@
       <c r="D8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6807,7 +6807,7 @@
       <c r="D9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6824,7 +6824,7 @@
       <c r="D10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6841,7 +6841,7 @@
       <c r="D11" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6858,7 +6858,7 @@
       <c r="D12" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6875,7 +6875,7 @@
       <c r="D13" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6892,7 +6892,7 @@
       <c r="D14" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6909,7 +6909,7 @@
       <c r="D15" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6926,7 +6926,7 @@
       <c r="D16" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6943,7 +6943,7 @@
       <c r="D17" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6960,7 +6960,7 @@
       <c r="D18" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6977,7 +6977,7 @@
       <c r="D19" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -6994,7 +6994,7 @@
       <c r="D20" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7011,7 +7011,7 @@
       <c r="D21" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7028,7 +7028,7 @@
       <c r="D22" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7045,7 +7045,7 @@
       <c r="D23" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7062,7 +7062,7 @@
       <c r="D24" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7079,7 +7079,7 @@
       <c r="D25" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7096,7 +7096,7 @@
       <c r="D26" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7113,7 +7113,7 @@
       <c r="D27" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7130,7 +7130,7 @@
       <c r="D28" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7147,7 +7147,7 @@
       <c r="D29" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7164,7 +7164,7 @@
       <c r="D30" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7181,7 +7181,7 @@
       <c r="D31" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7198,7 +7198,7 @@
       <c r="D32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7215,7 +7215,7 @@
       <c r="D33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7232,7 +7232,7 @@
       <c r="D34" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7249,7 +7249,7 @@
       <c r="D35" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7266,7 +7266,7 @@
       <c r="D36" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7283,7 +7283,7 @@
       <c r="D37" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7300,7 +7300,7 @@
       <c r="D38" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7317,7 +7317,7 @@
       <c r="D39" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7339,8 +7339,8 @@
   </sheetPr>
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7362,7 +7362,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7379,7 +7379,7 @@
       <c r="D2" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7396,7 +7396,7 @@
       <c r="D3" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7413,7 +7413,7 @@
       <c r="D4" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7430,7 +7430,7 @@
       <c r="D5" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7447,7 +7447,7 @@
       <c r="D6" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7464,7 +7464,7 @@
       <c r="D7" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7481,7 +7481,7 @@
       <c r="D8" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7498,7 +7498,7 @@
       <c r="D9" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7512,7 +7512,7 @@
       <c r="D10" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7526,7 +7526,7 @@
       <c r="D11" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7543,7 +7543,7 @@
       <c r="D12" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7560,7 +7560,7 @@
       <c r="D13" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7577,7 +7577,7 @@
       <c r="D14" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7594,7 +7594,7 @@
       <c r="D15" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7611,7 +7611,7 @@
       <c r="D16" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7628,7 +7628,7 @@
       <c r="D17" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7645,7 +7645,7 @@
       <c r="D18" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7662,7 +7662,7 @@
       <c r="D19" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7679,7 +7679,7 @@
       <c r="D20" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7696,7 +7696,7 @@
       <c r="D21" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7713,7 +7713,7 @@
       <c r="D22" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7730,7 +7730,7 @@
       <c r="D23" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7747,7 +7747,7 @@
       <c r="D24" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7764,7 +7764,7 @@
       <c r="D25" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7781,7 +7781,7 @@
       <c r="D26" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -7798,7 +7798,7 @@
       <c r="D27" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7815,7 +7815,7 @@
       <c r="D28" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7832,7 +7832,7 @@
       <c r="D29" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7849,7 +7849,7 @@
       <c r="D30" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7866,7 +7866,7 @@
       <c r="D31" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7883,7 +7883,7 @@
       <c r="D32" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7900,7 +7900,7 @@
       <c r="D33" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7917,7 +7917,7 @@
       <c r="D34" s="1" t="s">
         <v>502</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7934,7 +7934,7 @@
       <c r="D35" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       <c r="D36" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7968,7 +7968,7 @@
       <c r="D37" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -7985,7 +7985,7 @@
       <c r="D38" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8002,7 +8002,7 @@
       <c r="D39" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8019,7 +8019,7 @@
       <c r="D40" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8036,7 +8036,7 @@
       <c r="D41" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8053,8 +8053,8 @@
       <c r="D42" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E42" s="0" t="n">
-        <v>20</v>
+      <c r="E42" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8070,8 +8070,8 @@
       <c r="D43" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E43" s="0" t="n">
-        <v>20</v>
+      <c r="E43" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8087,8 +8087,8 @@
       <c r="D44" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E44" s="0" t="n">
-        <v>20</v>
+      <c r="E44" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8104,8 +8104,8 @@
       <c r="D45" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E45" s="0" t="n">
-        <v>20</v>
+      <c r="E45" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8121,8 +8121,8 @@
       <c r="D46" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E46" s="0" t="n">
-        <v>20</v>
+      <c r="E46" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8138,8 +8138,8 @@
       <c r="D47" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E47" s="0" t="n">
-        <v>20</v>
+      <c r="E47" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8155,8 +8155,8 @@
       <c r="D48" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E48" s="0" t="n">
-        <v>20</v>
+      <c r="E48" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8172,8 +8172,8 @@
       <c r="D49" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E49" s="0" t="n">
-        <v>20</v>
+      <c r="E49" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8189,8 +8189,8 @@
       <c r="D50" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E50" s="0" t="n">
-        <v>20</v>
+      <c r="E50" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8206,8 +8206,8 @@
       <c r="D51" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E51" s="0" t="n">
-        <v>20</v>
+      <c r="E51" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -8251,7 +8251,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8268,7 +8268,7 @@
       <c r="D2" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8285,7 +8285,7 @@
       <c r="D3" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8302,7 +8302,7 @@
       <c r="D4" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8319,7 +8319,7 @@
       <c r="D5" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8336,7 +8336,7 @@
       <c r="D6" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8353,7 +8353,7 @@
       <c r="D7" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8370,7 +8370,7 @@
       <c r="D8" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8387,7 +8387,7 @@
       <c r="D9" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8404,7 +8404,7 @@
       <c r="D10" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8421,7 +8421,7 @@
       <c r="D11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8438,7 +8438,7 @@
       <c r="D12" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8455,7 +8455,7 @@
       <c r="D13" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8472,7 +8472,7 @@
       <c r="D14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8489,7 +8489,7 @@
       <c r="D15" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8506,7 +8506,7 @@
       <c r="D16" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8523,7 +8523,7 @@
       <c r="D17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8540,7 +8540,7 @@
       <c r="D18" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8557,7 +8557,7 @@
       <c r="D19" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8574,7 +8574,7 @@
       <c r="D20" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8591,7 +8591,7 @@
       <c r="D21" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8608,7 +8608,7 @@
       <c r="D22" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8625,7 +8625,7 @@
       <c r="D23" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8642,7 +8642,7 @@
       <c r="D24" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8659,7 +8659,7 @@
       <c r="D25" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8676,7 +8676,7 @@
       <c r="D26" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8693,7 +8693,7 @@
       <c r="D27" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8710,7 +8710,7 @@
       <c r="D28" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8727,7 +8727,7 @@
       <c r="D29" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8744,7 +8744,7 @@
       <c r="D30" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8761,7 +8761,7 @@
       <c r="D31" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8778,7 +8778,7 @@
       <c r="D32" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8795,7 +8795,7 @@
       <c r="D33" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8812,7 +8812,7 @@
       <c r="D34" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
       <c r="D35" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8846,7 +8846,7 @@
       <c r="D36" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8863,7 +8863,7 @@
       <c r="D37" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8880,7 +8880,7 @@
       <c r="D38" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8897,7 +8897,7 @@
       <c r="D39" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8914,7 +8914,7 @@
       <c r="D40" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8931,7 +8931,7 @@
       <c r="D41" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8948,7 +8948,7 @@
       <c r="D42" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -8993,7 +8993,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9010,7 +9010,7 @@
       <c r="D2" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9027,7 +9027,7 @@
       <c r="D3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9044,7 +9044,7 @@
       <c r="D4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9061,7 +9061,7 @@
       <c r="D5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9078,7 +9078,7 @@
       <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9095,7 +9095,7 @@
       <c r="D7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9112,7 +9112,7 @@
       <c r="D8" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9129,7 +9129,7 @@
       <c r="D9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9146,7 +9146,7 @@
       <c r="D10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9163,7 +9163,7 @@
       <c r="D11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9180,7 +9180,7 @@
       <c r="D12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9197,7 +9197,7 @@
       <c r="D13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9214,7 +9214,7 @@
       <c r="D14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9231,7 +9231,7 @@
       <c r="D15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9248,7 +9248,7 @@
       <c r="D16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9265,7 +9265,7 @@
       <c r="D17" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9282,7 +9282,7 @@
       <c r="D18" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9299,7 +9299,7 @@
       <c r="D19" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9316,7 +9316,7 @@
       <c r="D20" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9333,7 +9333,7 @@
       <c r="D21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9350,7 +9350,7 @@
       <c r="D22" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9367,7 +9367,7 @@
       <c r="D23" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9384,7 +9384,7 @@
       <c r="D24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9401,7 +9401,7 @@
       <c r="D25" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9418,7 +9418,7 @@
       <c r="D26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9435,7 +9435,7 @@
       <c r="D27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9452,7 +9452,7 @@
       <c r="D28" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9469,7 +9469,7 @@
       <c r="D29" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9486,7 +9486,7 @@
       <c r="D30" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9503,7 +9503,7 @@
       <c r="D31" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9520,7 +9520,7 @@
       <c r="D32" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9537,7 +9537,7 @@
       <c r="D33" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9552,7 +9552,7 @@
       <c r="D34" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9569,7 +9569,7 @@
       <c r="D35" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9586,7 +9586,7 @@
       <c r="D36" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9603,7 +9603,7 @@
       <c r="D37" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9620,7 +9620,7 @@
       <c r="D38" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9637,7 +9637,7 @@
       <c r="D39" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9654,7 +9654,7 @@
       <c r="D40" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9671,7 +9671,7 @@
       <c r="D41" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9688,7 +9688,7 @@
       <c r="D42" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9705,7 +9705,7 @@
       <c r="D43" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9722,7 +9722,7 @@
       <c r="D44" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9739,7 +9739,7 @@
       <c r="D45" s="1" t="s">
         <v>706</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9756,7 +9756,7 @@
       <c r="D46" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       <c r="D47" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9790,7 +9790,7 @@
       <c r="D48" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9807,7 +9807,7 @@
       <c r="D49" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9824,7 +9824,7 @@
       <c r="D50" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9841,7 +9841,7 @@
       <c r="D51" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9858,7 +9858,7 @@
       <c r="D52" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9875,7 +9875,7 @@
       <c r="D53" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9892,7 +9892,7 @@
       <c r="D54" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9909,7 +9909,7 @@
       <c r="D55" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9926,7 +9926,7 @@
       <c r="D56" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="E56" s="0" t="n">
+      <c r="E56" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9943,7 +9943,7 @@
       <c r="D57" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9960,7 +9960,7 @@
       <c r="D58" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9977,7 +9977,7 @@
       <c r="D59" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -9994,7 +9994,7 @@
       <c r="D60" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10011,7 +10011,7 @@
       <c r="D61" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10028,7 +10028,7 @@
       <c r="D62" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10045,7 +10045,7 @@
       <c r="D63" s="1" t="s">
         <v>754</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10062,7 +10062,7 @@
       <c r="D64" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E64" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10079,7 +10079,7 @@
       <c r="D65" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E65" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10096,7 +10096,7 @@
       <c r="D66" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10113,7 +10113,7 @@
       <c r="D67" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10130,7 +10130,7 @@
       <c r="D68" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10147,7 +10147,7 @@
       <c r="D69" s="1" t="s">
         <v>768</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10164,7 +10164,7 @@
       <c r="D70" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -10209,7 +10209,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -10226,7 +10226,7 @@
       <c r="D2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10243,7 +10243,7 @@
       <c r="D3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10260,7 +10260,7 @@
       <c r="D4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10277,7 +10277,7 @@
       <c r="D5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10294,7 +10294,7 @@
       <c r="D6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10311,7 +10311,7 @@
       <c r="D7" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10328,7 +10328,7 @@
       <c r="D8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10345,7 +10345,7 @@
       <c r="D9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10362,7 +10362,7 @@
       <c r="D10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10379,7 +10379,7 @@
       <c r="D11" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10396,7 +10396,7 @@
       <c r="D12" s="1" t="s">
         <v>669</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10413,7 +10413,7 @@
       <c r="D13" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10430,7 +10430,7 @@
       <c r="D14" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10447,7 +10447,7 @@
       <c r="D15" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10464,7 +10464,7 @@
       <c r="D16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10481,7 +10481,7 @@
       <c r="D17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10498,7 +10498,7 @@
       <c r="D18" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10515,7 +10515,7 @@
       <c r="D19" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10532,7 +10532,7 @@
       <c r="D20" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10549,7 +10549,7 @@
       <c r="D21" s="1" t="s">
         <v>816</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10566,7 +10566,7 @@
       <c r="D22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10583,7 +10583,7 @@
       <c r="D23" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10600,7 +10600,7 @@
       <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10617,7 +10617,7 @@
       <c r="D25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10634,7 +10634,7 @@
       <c r="D26" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10651,7 +10651,7 @@
       <c r="D27" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10668,7 +10668,7 @@
       <c r="D28" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10685,7 +10685,7 @@
       <c r="D29" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10702,7 +10702,7 @@
       <c r="D30" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10719,7 +10719,7 @@
       <c r="D31" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10736,7 +10736,7 @@
       <c r="D32" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10753,7 +10753,7 @@
       <c r="D33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10770,7 +10770,7 @@
       <c r="D34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10787,7 +10787,7 @@
       <c r="D35" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10804,7 +10804,7 @@
       <c r="D36" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10821,7 +10821,7 @@
       <c r="D37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10838,7 +10838,7 @@
       <c r="D38" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10855,7 +10855,7 @@
       <c r="D39" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10872,7 +10872,7 @@
       <c r="D40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10889,7 +10889,7 @@
       <c r="D41" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10906,7 +10906,7 @@
       <c r="D42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10923,7 +10923,7 @@
       <c r="D43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10940,7 +10940,7 @@
       <c r="D44" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10957,7 +10957,7 @@
       <c r="D45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10974,7 +10974,7 @@
       <c r="D46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -10991,7 +10991,7 @@
       <c r="D47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11008,7 +11008,7 @@
       <c r="D48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11025,7 +11025,7 @@
       <c r="D49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11042,7 +11042,7 @@
       <c r="D50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11059,7 +11059,7 @@
       <c r="D51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="1" t="n">
         <v>20</v>
       </c>
     </row>
@@ -11081,7 +11081,7 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -11104,7 +11104,7 @@
       <c r="D1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11121,7 +11121,7 @@
       <c r="D2" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11138,7 +11138,7 @@
       <c r="D3" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11155,7 +11155,7 @@
       <c r="D4" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11172,7 +11172,7 @@
       <c r="D5" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11189,7 +11189,7 @@
       <c r="D6" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11206,7 +11206,7 @@
       <c r="D7" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11223,7 +11223,7 @@
       <c r="D8" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11240,7 +11240,7 @@
       <c r="D9" s="1" t="s">
         <v>878</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11257,7 +11257,7 @@
       <c r="D10" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11274,7 +11274,7 @@
       <c r="D11" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11291,7 +11291,7 @@
       <c r="D12" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11308,7 +11308,7 @@
       <c r="D13" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11325,7 +11325,7 @@
       <c r="D14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11342,7 +11342,7 @@
       <c r="D15" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11359,7 +11359,7 @@
       <c r="D16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11376,7 +11376,7 @@
       <c r="D17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11393,7 +11393,7 @@
       <c r="D18" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11410,7 +11410,7 @@
       <c r="D19" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>10</v>
       </c>
     </row>
@@ -11427,7 +11427,7 @@
       <c r="D20" s="1" t="s">
         <v>895</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>